<commit_message>
Update batch prep file
</commit_message>
<xml_diff>
--- a/data_files/Example/Input/example_rates.xlsx
+++ b/data_files/Example/Input/example_rates.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeichman\Documents\gamsdir\projdir\RODeO\data_files\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeichman\Documents\gamsdir\projdir\RODeO\data_files\Example\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>58fa647a5457a38f40156660</t>
   </si>
@@ -75,6 +75,21 @@
   </si>
   <si>
     <t>58fa71745457a35245156661</t>
+  </si>
+  <si>
+    <t>586fd4265457a306691c9607</t>
+  </si>
+  <si>
+    <t>587016a85457a3d7241c9605</t>
+  </si>
+  <si>
+    <t>587932be5457a3b25fdda4d6</t>
+  </si>
+  <si>
+    <t>587e43145457a37c4c316ce6</t>
+  </si>
+  <si>
+    <t>587e9b805457a3d855316ce6</t>
   </si>
 </sst>
 </file>
@@ -110,8 +125,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,98 +442,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F265C9-E19E-47E6-97AC-CD8B0A6F7144}">
-  <dimension ref="A1:A17"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
+      <c r="A5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A1:A22">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>